<commit_message>
Changed a file name based on failed File Match check
</commit_message>
<xml_diff>
--- a/villegas/OLR/OLR_villegas_mss0758.xlsx
+++ b/villegas/OLR/OLR_villegas_mss0758.xlsx
@@ -2148,9 +2148,6 @@
     <t>m0758b03f016</t>
   </si>
   <si>
-    <t>m0758b03f016.tiff</t>
-  </si>
-  <si>
     <t>1885-09-02</t>
   </si>
   <si>
@@ -2635,6 +2632,9 @@
   </si>
   <si>
     <t>Broadsides</t>
+  </si>
+  <si>
+    <t>m0758b03f016.tif</t>
   </si>
 </sst>
 </file>
@@ -3681,7 +3681,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B2" sqref="B2"/>
+      <selection pane="bottomLeft" activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3804,17 +3804,17 @@
       </c>
       <c r="K2" s="24"/>
       <c r="L2" s="24" t="s">
-        <v>800</v>
+        <v>799</v>
       </c>
       <c r="M2" s="24" t="s">
+        <v>829</v>
+      </c>
+      <c r="N2" s="24" t="s">
         <v>830</v>
-      </c>
-      <c r="N2" s="24" t="s">
-        <v>831</v>
       </c>
       <c r="O2" s="24"/>
       <c r="P2" s="25" t="s">
-        <v>811</v>
+        <v>810</v>
       </c>
       <c r="Q2" s="24"/>
       <c r="R2" s="24" t="s">
@@ -3828,12 +3828,12 @@
       </c>
       <c r="U2" s="24"/>
       <c r="V2" s="24" t="s">
-        <v>801</v>
+        <v>800</v>
       </c>
       <c r="W2" s="24"/>
       <c r="X2" s="24"/>
       <c r="Y2" s="24" t="s">
-        <v>802</v>
+        <v>801</v>
       </c>
     </row>
     <row r="3" spans="1:25" x14ac:dyDescent="0.25">
@@ -3841,7 +3841,7 @@
         <v>632</v>
       </c>
       <c r="B3" t="s">
-        <v>828</v>
+        <v>827</v>
       </c>
       <c r="C3" t="s">
         <v>634</v>
@@ -3884,7 +3884,7 @@
         <v>632</v>
       </c>
       <c r="B4" t="s">
-        <v>828</v>
+        <v>827</v>
       </c>
       <c r="C4" t="s">
         <v>635</v>
@@ -3954,21 +3954,21 @@
         <v>658</v>
       </c>
       <c r="K5" s="24" t="s">
-        <v>808</v>
+        <v>807</v>
       </c>
       <c r="L5" s="24" t="s">
         <v>646</v>
       </c>
       <c r="M5" s="24" t="s">
-        <v>754</v>
+        <v>753</v>
       </c>
       <c r="N5" s="24" t="s">
-        <v>756</v>
+        <v>755</v>
       </c>
       <c r="O5" s="24"/>
       <c r="P5" s="24"/>
       <c r="Q5" s="24" t="s">
-        <v>798</v>
+        <v>797</v>
       </c>
       <c r="R5" s="24" t="s">
         <v>647</v>
@@ -3983,14 +3983,14 @@
         <v>648</v>
       </c>
       <c r="V5" s="24" t="s">
-        <v>801</v>
+        <v>800</v>
       </c>
       <c r="W5" s="24" t="s">
-        <v>808</v>
+        <v>807</v>
       </c>
       <c r="X5" s="24"/>
       <c r="Y5" s="24" t="s">
-        <v>803</v>
+        <v>802</v>
       </c>
     </row>
     <row r="6" spans="1:25" x14ac:dyDescent="0.25">
@@ -4016,23 +4016,23 @@
       </c>
       <c r="I6" s="24"/>
       <c r="J6" s="24" t="s">
-        <v>817</v>
+        <v>816</v>
       </c>
       <c r="K6" s="24"/>
       <c r="L6" s="24" t="s">
+        <v>811</v>
+      </c>
+      <c r="M6" s="24" t="s">
         <v>812</v>
       </c>
-      <c r="M6" s="24" t="s">
+      <c r="N6" s="24" t="s">
         <v>813</v>
       </c>
-      <c r="N6" s="24" t="s">
-        <v>814</v>
-      </c>
       <c r="O6" s="24" t="s">
-        <v>823</v>
+        <v>822</v>
       </c>
       <c r="P6" s="25" t="s">
-        <v>816</v>
+        <v>815</v>
       </c>
       <c r="Q6" s="24"/>
       <c r="R6" s="24" t="s">
@@ -4048,14 +4048,14 @@
         <v>652</v>
       </c>
       <c r="V6" s="24" t="s">
-        <v>801</v>
+        <v>800</v>
       </c>
       <c r="W6" s="24" t="s">
-        <v>808</v>
+        <v>807</v>
       </c>
       <c r="X6" s="24"/>
       <c r="Y6" s="24" t="s">
-        <v>807</v>
+        <v>806</v>
       </c>
     </row>
     <row r="7" spans="1:25" x14ac:dyDescent="0.25">
@@ -4081,23 +4081,23 @@
       </c>
       <c r="I7" s="24"/>
       <c r="J7" s="24" t="s">
-        <v>818</v>
+        <v>817</v>
       </c>
       <c r="K7" s="24"/>
       <c r="L7" s="24" t="s">
+        <v>811</v>
+      </c>
+      <c r="M7" s="24" t="s">
         <v>812</v>
       </c>
-      <c r="M7" s="24" t="s">
+      <c r="N7" s="24" t="s">
         <v>813</v>
       </c>
-      <c r="N7" s="24" t="s">
-        <v>814</v>
-      </c>
       <c r="O7" s="24" t="s">
-        <v>796</v>
+        <v>795</v>
       </c>
       <c r="P7" s="25" t="s">
-        <v>816</v>
+        <v>815</v>
       </c>
       <c r="Q7" s="24"/>
       <c r="R7" s="24" t="s">
@@ -4113,14 +4113,14 @@
         <v>653</v>
       </c>
       <c r="V7" s="24" t="s">
-        <v>801</v>
+        <v>800</v>
       </c>
       <c r="W7" s="24" t="s">
-        <v>808</v>
+        <v>807</v>
       </c>
       <c r="X7" s="24"/>
       <c r="Y7" s="24" t="s">
-        <v>807</v>
+        <v>806</v>
       </c>
     </row>
     <row r="8" spans="1:25" x14ac:dyDescent="0.25">
@@ -4146,23 +4146,23 @@
       </c>
       <c r="I8" s="26"/>
       <c r="J8" s="26" t="s">
-        <v>819</v>
+        <v>818</v>
       </c>
       <c r="K8" s="24"/>
       <c r="L8" s="24" t="s">
+        <v>811</v>
+      </c>
+      <c r="M8" s="24" t="s">
         <v>812</v>
       </c>
-      <c r="M8" s="24" t="s">
+      <c r="N8" s="24" t="s">
         <v>813</v>
       </c>
-      <c r="N8" s="24" t="s">
-        <v>814</v>
-      </c>
       <c r="O8" s="26" t="s">
-        <v>797</v>
+        <v>796</v>
       </c>
       <c r="P8" s="25" t="s">
-        <v>816</v>
+        <v>815</v>
       </c>
       <c r="Q8" s="26"/>
       <c r="R8" s="24" t="s">
@@ -4178,14 +4178,14 @@
         <v>654</v>
       </c>
       <c r="V8" s="24" t="s">
-        <v>801</v>
+        <v>800</v>
       </c>
       <c r="W8" s="24" t="s">
-        <v>808</v>
+        <v>807</v>
       </c>
       <c r="X8" s="24"/>
       <c r="Y8" s="24" t="s">
-        <v>807</v>
+        <v>806</v>
       </c>
     </row>
     <row r="9" spans="1:25" x14ac:dyDescent="0.25">
@@ -4215,19 +4215,19 @@
       </c>
       <c r="K9" s="24"/>
       <c r="L9" s="24" t="s">
+        <v>811</v>
+      </c>
+      <c r="M9" s="24" t="s">
         <v>812</v>
       </c>
-      <c r="M9" s="24" t="s">
+      <c r="N9" s="24" t="s">
         <v>813</v>
       </c>
-      <c r="N9" s="24" t="s">
+      <c r="O9" s="27" t="s">
+        <v>823</v>
+      </c>
+      <c r="P9" s="25" t="s">
         <v>814</v>
-      </c>
-      <c r="O9" s="27" t="s">
-        <v>824</v>
-      </c>
-      <c r="P9" s="25" t="s">
-        <v>815</v>
       </c>
       <c r="Q9" s="27"/>
       <c r="R9" s="24" t="s">
@@ -4243,14 +4243,14 @@
         <v>665</v>
       </c>
       <c r="V9" s="24" t="s">
-        <v>801</v>
+        <v>800</v>
       </c>
       <c r="W9" s="24" t="s">
-        <v>808</v>
+        <v>807</v>
       </c>
       <c r="X9" s="24"/>
       <c r="Y9" s="24" t="s">
-        <v>807</v>
+        <v>806</v>
       </c>
     </row>
     <row r="10" spans="1:25" x14ac:dyDescent="0.25">
@@ -4276,23 +4276,23 @@
       </c>
       <c r="I10" s="26"/>
       <c r="J10" s="12" t="s">
-        <v>820</v>
+        <v>819</v>
       </c>
       <c r="K10" s="24"/>
       <c r="L10" s="24" t="s">
+        <v>811</v>
+      </c>
+      <c r="M10" s="24" t="s">
         <v>812</v>
       </c>
-      <c r="M10" s="24" t="s">
+      <c r="N10" s="24" t="s">
         <v>813</v>
       </c>
-      <c r="N10" s="24" t="s">
+      <c r="O10" s="27" t="s">
+        <v>824</v>
+      </c>
+      <c r="P10" s="25" t="s">
         <v>814</v>
-      </c>
-      <c r="O10" s="27" t="s">
-        <v>825</v>
-      </c>
-      <c r="P10" s="25" t="s">
-        <v>815</v>
       </c>
       <c r="Q10" s="27"/>
       <c r="R10" s="24" t="s">
@@ -4308,14 +4308,14 @@
         <v>666</v>
       </c>
       <c r="V10" s="24" t="s">
-        <v>805</v>
+        <v>804</v>
       </c>
       <c r="W10" s="24" t="s">
-        <v>808</v>
+        <v>807</v>
       </c>
       <c r="X10" s="24"/>
       <c r="Y10" s="24" t="s">
-        <v>807</v>
+        <v>806</v>
       </c>
     </row>
     <row r="11" spans="1:25" x14ac:dyDescent="0.25">
@@ -4332,7 +4332,7 @@
         <v>384</v>
       </c>
       <c r="E11" s="24" t="s">
-        <v>671</v>
+        <v>833</v>
       </c>
       <c r="F11" s="24" t="s">
         <v>381</v>
@@ -4345,22 +4345,22 @@
       </c>
       <c r="I11" s="24"/>
       <c r="J11" s="24" t="s">
-        <v>792</v>
+        <v>791</v>
       </c>
       <c r="K11" s="24"/>
       <c r="L11" s="24" t="s">
         <v>668</v>
       </c>
       <c r="M11" s="24" t="s">
-        <v>672</v>
+        <v>671</v>
       </c>
       <c r="N11" s="24" t="s">
-        <v>672</v>
+        <v>671</v>
       </c>
       <c r="O11" s="24"/>
       <c r="P11" s="24"/>
       <c r="Q11" s="24" t="s">
-        <v>793</v>
+        <v>792</v>
       </c>
       <c r="R11" s="24" t="s">
         <v>647</v>
@@ -4377,27 +4377,27 @@
       <c r="V11" s="24"/>
       <c r="W11" s="24"/>
       <c r="X11" s="24" t="s">
-        <v>833</v>
+        <v>832</v>
       </c>
       <c r="Y11" s="24" t="s">
-        <v>803</v>
+        <v>802</v>
       </c>
     </row>
     <row r="12" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A12" s="24" t="s">
-        <v>673</v>
+        <v>672</v>
       </c>
       <c r="B12" s="28" t="s">
         <v>485</v>
       </c>
       <c r="C12" s="24" t="s">
-        <v>675</v>
+        <v>674</v>
       </c>
       <c r="D12" s="24" t="s">
         <v>384</v>
       </c>
       <c r="E12" s="24" t="s">
-        <v>676</v>
+        <v>675</v>
       </c>
       <c r="F12" s="24" t="s">
         <v>381</v>
@@ -4412,27 +4412,27 @@
         <v>433</v>
       </c>
       <c r="J12" s="24" t="s">
+        <v>676</v>
+      </c>
+      <c r="K12" s="24" t="s">
+        <v>807</v>
+      </c>
+      <c r="L12" s="24" t="s">
         <v>677</v>
       </c>
-      <c r="K12" s="24" t="s">
-        <v>808</v>
-      </c>
-      <c r="L12" s="24" t="s">
-        <v>678</v>
-      </c>
       <c r="M12" s="24" t="s">
+        <v>750</v>
+      </c>
+      <c r="N12" s="24" t="s">
         <v>751</v>
-      </c>
-      <c r="N12" s="24" t="s">
-        <v>752</v>
       </c>
       <c r="O12" s="24"/>
       <c r="P12" s="24"/>
       <c r="Q12" s="24" t="s">
-        <v>753</v>
+        <v>752</v>
       </c>
       <c r="R12" s="24" t="s">
-        <v>687</v>
+        <v>686</v>
       </c>
       <c r="S12" s="24" t="s">
         <v>641</v>
@@ -4441,34 +4441,34 @@
         <v>642</v>
       </c>
       <c r="U12" s="24" t="s">
-        <v>674</v>
+        <v>673</v>
       </c>
       <c r="V12" s="24" t="s">
-        <v>801</v>
+        <v>800</v>
       </c>
       <c r="W12" s="24" t="s">
-        <v>808</v>
+        <v>807</v>
       </c>
       <c r="X12" s="24"/>
       <c r="Y12" s="24" t="s">
-        <v>803</v>
+        <v>802</v>
       </c>
     </row>
     <row r="13" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A13" s="24" t="s">
-        <v>679</v>
+        <v>678</v>
       </c>
       <c r="B13" s="28" t="s">
         <v>485</v>
       </c>
       <c r="C13" s="24" t="s">
-        <v>680</v>
+        <v>679</v>
       </c>
       <c r="D13" s="24" t="s">
         <v>384</v>
       </c>
       <c r="E13" s="24" t="s">
-        <v>682</v>
+        <v>681</v>
       </c>
       <c r="F13" s="24" t="s">
         <v>381</v>
@@ -4481,27 +4481,27 @@
       </c>
       <c r="I13" s="24"/>
       <c r="J13" s="25" t="s">
-        <v>681</v>
+        <v>680</v>
       </c>
       <c r="K13" s="24" t="s">
-        <v>808</v>
+        <v>807</v>
       </c>
       <c r="L13" s="24" t="s">
+        <v>683</v>
+      </c>
+      <c r="M13" s="24" t="s">
         <v>684</v>
       </c>
-      <c r="M13" s="24" t="s">
-        <v>685</v>
-      </c>
       <c r="N13" s="24" t="s">
-        <v>685</v>
+        <v>684</v>
       </c>
       <c r="O13" s="24"/>
       <c r="P13" s="24"/>
       <c r="Q13" s="24" t="s">
-        <v>755</v>
+        <v>754</v>
       </c>
       <c r="R13" s="24" t="s">
-        <v>687</v>
+        <v>686</v>
       </c>
       <c r="S13" s="24" t="s">
         <v>641</v>
@@ -4510,34 +4510,34 @@
         <v>642</v>
       </c>
       <c r="U13" s="24" t="s">
-        <v>688</v>
+        <v>687</v>
       </c>
       <c r="V13" s="24" t="s">
-        <v>801</v>
+        <v>800</v>
       </c>
       <c r="W13" s="24" t="s">
-        <v>808</v>
+        <v>807</v>
       </c>
       <c r="X13" s="24"/>
       <c r="Y13" s="24" t="s">
-        <v>803</v>
+        <v>802</v>
       </c>
     </row>
     <row r="14" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A14" s="24" t="s">
-        <v>683</v>
+        <v>682</v>
       </c>
       <c r="B14" s="28" t="s">
         <v>485</v>
       </c>
       <c r="C14" s="24" t="s">
-        <v>686</v>
+        <v>685</v>
       </c>
       <c r="D14" s="24" t="s">
         <v>384</v>
       </c>
       <c r="E14" s="24" t="s">
-        <v>829</v>
+        <v>828</v>
       </c>
       <c r="F14" s="24" t="s">
         <v>381</v>
@@ -4552,27 +4552,27 @@
         <v>358</v>
       </c>
       <c r="J14" s="24" t="s">
-        <v>677</v>
+        <v>676</v>
       </c>
       <c r="K14" s="24" t="s">
-        <v>808</v>
+        <v>807</v>
       </c>
       <c r="L14" s="24" t="s">
+        <v>757</v>
+      </c>
+      <c r="M14" s="24" t="s">
+        <v>756</v>
+      </c>
+      <c r="N14" s="24" t="s">
         <v>758</v>
-      </c>
-      <c r="M14" s="24" t="s">
-        <v>757</v>
-      </c>
-      <c r="N14" s="24" t="s">
-        <v>759</v>
       </c>
       <c r="O14" s="24"/>
       <c r="P14" s="24"/>
       <c r="Q14" s="24" t="s">
-        <v>760</v>
+        <v>759</v>
       </c>
       <c r="R14" s="24" t="s">
-        <v>687</v>
+        <v>686</v>
       </c>
       <c r="S14" s="24" t="s">
         <v>641</v>
@@ -4581,34 +4581,34 @@
         <v>642</v>
       </c>
       <c r="U14" s="24" t="s">
-        <v>689</v>
+        <v>688</v>
       </c>
       <c r="V14" s="24" t="s">
-        <v>801</v>
+        <v>800</v>
       </c>
       <c r="W14" s="24" t="s">
-        <v>808</v>
+        <v>807</v>
       </c>
       <c r="X14" s="24"/>
       <c r="Y14" s="24" t="s">
-        <v>803</v>
+        <v>802</v>
       </c>
     </row>
     <row r="15" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A15" s="24" t="s">
-        <v>690</v>
+        <v>689</v>
       </c>
       <c r="B15" s="28" t="s">
         <v>485</v>
       </c>
       <c r="C15" s="24" t="s">
-        <v>693</v>
+        <v>692</v>
       </c>
       <c r="D15" s="24" t="s">
         <v>384</v>
       </c>
       <c r="E15" s="24" t="s">
-        <v>696</v>
+        <v>695</v>
       </c>
       <c r="F15" s="24" t="s">
         <v>381</v>
@@ -4623,27 +4623,27 @@
         <v>358</v>
       </c>
       <c r="J15" s="24" t="s">
-        <v>677</v>
+        <v>676</v>
       </c>
       <c r="K15" s="24" t="s">
-        <v>808</v>
+        <v>807</v>
       </c>
       <c r="L15" s="24" t="s">
-        <v>766</v>
+        <v>765</v>
       </c>
       <c r="M15" s="24" t="s">
-        <v>765</v>
+        <v>764</v>
       </c>
       <c r="N15" s="24" t="s">
-        <v>832</v>
+        <v>831</v>
       </c>
       <c r="O15" s="24"/>
       <c r="P15" s="24"/>
       <c r="Q15" s="24" t="s">
-        <v>767</v>
+        <v>766</v>
       </c>
       <c r="R15" s="24" t="s">
-        <v>687</v>
+        <v>686</v>
       </c>
       <c r="S15" s="24" t="s">
         <v>641</v>
@@ -4652,34 +4652,34 @@
         <v>642</v>
       </c>
       <c r="U15" s="24" t="s">
-        <v>699</v>
+        <v>698</v>
       </c>
       <c r="V15" s="24" t="s">
-        <v>801</v>
+        <v>800</v>
       </c>
       <c r="W15" s="24" t="s">
-        <v>808</v>
+        <v>807</v>
       </c>
       <c r="X15" s="24"/>
       <c r="Y15" s="24" t="s">
-        <v>803</v>
+        <v>802</v>
       </c>
     </row>
     <row r="16" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A16" s="24" t="s">
-        <v>691</v>
+        <v>690</v>
       </c>
       <c r="B16" s="28" t="s">
         <v>485</v>
       </c>
       <c r="C16" s="24" t="s">
-        <v>694</v>
+        <v>693</v>
       </c>
       <c r="D16" s="24" t="s">
         <v>384</v>
       </c>
       <c r="E16" s="24" t="s">
-        <v>697</v>
+        <v>696</v>
       </c>
       <c r="F16" s="24" t="s">
         <v>381</v>
@@ -4694,27 +4694,27 @@
         <v>358</v>
       </c>
       <c r="J16" s="24" t="s">
-        <v>677</v>
+        <v>676</v>
       </c>
       <c r="K16" s="24" t="s">
-        <v>808</v>
+        <v>807</v>
       </c>
       <c r="L16" s="24" t="s">
+        <v>761</v>
+      </c>
+      <c r="M16" s="24" t="s">
+        <v>760</v>
+      </c>
+      <c r="N16" s="24" t="s">
         <v>762</v>
-      </c>
-      <c r="M16" s="24" t="s">
-        <v>761</v>
-      </c>
-      <c r="N16" s="24" t="s">
-        <v>763</v>
       </c>
       <c r="O16" s="24"/>
       <c r="P16" s="24"/>
       <c r="Q16" s="24" t="s">
-        <v>764</v>
+        <v>763</v>
       </c>
       <c r="R16" s="24" t="s">
-        <v>687</v>
+        <v>686</v>
       </c>
       <c r="S16" s="24" t="s">
         <v>641</v>
@@ -4723,34 +4723,34 @@
         <v>642</v>
       </c>
       <c r="U16" s="24" t="s">
-        <v>700</v>
+        <v>699</v>
       </c>
       <c r="V16" s="24" t="s">
-        <v>801</v>
+        <v>800</v>
       </c>
       <c r="W16" s="24" t="s">
-        <v>808</v>
+        <v>807</v>
       </c>
       <c r="X16" s="24"/>
       <c r="Y16" s="24" t="s">
-        <v>803</v>
+        <v>802</v>
       </c>
     </row>
     <row r="17" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A17" s="24" t="s">
-        <v>692</v>
+        <v>691</v>
       </c>
       <c r="B17" s="28" t="s">
         <v>485</v>
       </c>
       <c r="C17" s="25" t="s">
-        <v>695</v>
+        <v>694</v>
       </c>
       <c r="D17" s="24" t="s">
         <v>384</v>
       </c>
       <c r="E17" s="24" t="s">
-        <v>698</v>
+        <v>697</v>
       </c>
       <c r="F17" s="24" t="s">
         <v>381</v>
@@ -4765,27 +4765,27 @@
         <v>358</v>
       </c>
       <c r="J17" s="24" t="s">
-        <v>677</v>
+        <v>676</v>
       </c>
       <c r="K17" s="24" t="s">
-        <v>808</v>
+        <v>807</v>
       </c>
       <c r="L17" s="24" t="s">
         <v>664</v>
       </c>
       <c r="M17" s="24" t="s">
+        <v>773</v>
+      </c>
+      <c r="N17" s="24" t="s">
         <v>774</v>
-      </c>
-      <c r="N17" s="24" t="s">
-        <v>775</v>
       </c>
       <c r="O17" s="24"/>
       <c r="P17" s="24"/>
       <c r="Q17" s="24" t="s">
-        <v>776</v>
+        <v>775</v>
       </c>
       <c r="R17" s="24" t="s">
-        <v>687</v>
+        <v>686</v>
       </c>
       <c r="S17" s="24" t="s">
         <v>641</v>
@@ -4794,34 +4794,34 @@
         <v>642</v>
       </c>
       <c r="U17" s="24" t="s">
-        <v>701</v>
+        <v>700</v>
       </c>
       <c r="V17" s="24" t="s">
-        <v>804</v>
+        <v>803</v>
       </c>
       <c r="W17" s="24" t="s">
-        <v>808</v>
+        <v>807</v>
       </c>
       <c r="X17" s="24"/>
       <c r="Y17" s="24" t="s">
-        <v>803</v>
+        <v>802</v>
       </c>
     </row>
     <row r="18" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A18" s="24" t="s">
-        <v>702</v>
+        <v>701</v>
       </c>
       <c r="B18" s="28" t="s">
         <v>485</v>
       </c>
       <c r="C18" s="24" t="s">
-        <v>704</v>
+        <v>703</v>
       </c>
       <c r="D18" s="24" t="s">
         <v>384</v>
       </c>
       <c r="E18" s="24" t="s">
-        <v>705</v>
+        <v>704</v>
       </c>
       <c r="F18" s="24" t="s">
         <v>381</v>
@@ -4836,27 +4836,27 @@
         <v>358</v>
       </c>
       <c r="J18" s="24" t="s">
-        <v>677</v>
+        <v>676</v>
       </c>
       <c r="K18" s="24" t="s">
-        <v>808</v>
+        <v>807</v>
       </c>
       <c r="L18" s="24" t="s">
-        <v>703</v>
+        <v>702</v>
       </c>
       <c r="M18" s="24" t="s">
+        <v>783</v>
+      </c>
+      <c r="N18" s="24" t="s">
         <v>784</v>
-      </c>
-      <c r="N18" s="24" t="s">
-        <v>785</v>
       </c>
       <c r="O18" s="24"/>
       <c r="P18" s="24"/>
       <c r="Q18" s="24" t="s">
-        <v>799</v>
+        <v>798</v>
       </c>
       <c r="R18" s="24" t="s">
-        <v>687</v>
+        <v>686</v>
       </c>
       <c r="S18" s="24" t="s">
         <v>641</v>
@@ -4865,34 +4865,34 @@
         <v>642</v>
       </c>
       <c r="U18" s="24" t="s">
-        <v>706</v>
+        <v>705</v>
       </c>
       <c r="V18" s="24" t="s">
-        <v>801</v>
+        <v>800</v>
       </c>
       <c r="W18" s="24" t="s">
-        <v>808</v>
+        <v>807</v>
       </c>
       <c r="X18" s="24"/>
       <c r="Y18" s="24" t="s">
-        <v>803</v>
+        <v>802</v>
       </c>
     </row>
     <row r="19" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A19" s="24" t="s">
-        <v>707</v>
+        <v>706</v>
       </c>
       <c r="B19" s="28" t="s">
         <v>485</v>
       </c>
       <c r="C19" s="24" t="s">
-        <v>710</v>
+        <v>709</v>
       </c>
       <c r="D19" s="24" t="s">
         <v>384</v>
       </c>
       <c r="E19" s="24" t="s">
-        <v>713</v>
+        <v>712</v>
       </c>
       <c r="F19" s="24" t="s">
         <v>381</v>
@@ -4907,27 +4907,27 @@
         <v>358</v>
       </c>
       <c r="J19" s="24" t="s">
-        <v>677</v>
+        <v>676</v>
       </c>
       <c r="K19" s="24" t="s">
-        <v>808</v>
+        <v>807</v>
       </c>
       <c r="L19" s="25" t="s">
-        <v>716</v>
+        <v>715</v>
       </c>
       <c r="M19" s="24" t="s">
+        <v>780</v>
+      </c>
+      <c r="N19" s="24" t="s">
         <v>781</v>
-      </c>
-      <c r="N19" s="24" t="s">
-        <v>782</v>
       </c>
       <c r="O19" s="24"/>
       <c r="P19" s="24"/>
       <c r="Q19" s="24" t="s">
-        <v>783</v>
+        <v>782</v>
       </c>
       <c r="R19" s="24" t="s">
-        <v>687</v>
+        <v>686</v>
       </c>
       <c r="S19" s="24" t="s">
         <v>641</v>
@@ -4936,34 +4936,34 @@
         <v>642</v>
       </c>
       <c r="U19" s="24" t="s">
-        <v>717</v>
+        <v>716</v>
       </c>
       <c r="V19" s="24" t="s">
-        <v>801</v>
+        <v>800</v>
       </c>
       <c r="W19" s="24" t="s">
-        <v>808</v>
+        <v>807</v>
       </c>
       <c r="X19" s="24"/>
       <c r="Y19" s="24" t="s">
-        <v>803</v>
+        <v>802</v>
       </c>
     </row>
     <row r="20" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A20" s="24" t="s">
-        <v>708</v>
+        <v>707</v>
       </c>
       <c r="B20" s="28" t="s">
         <v>485</v>
       </c>
       <c r="C20" s="24" t="s">
-        <v>711</v>
+        <v>710</v>
       </c>
       <c r="D20" s="24" t="s">
         <v>384</v>
       </c>
       <c r="E20" s="24" t="s">
-        <v>714</v>
+        <v>713</v>
       </c>
       <c r="F20" s="24" t="s">
         <v>381</v>
@@ -4976,27 +4976,27 @@
       </c>
       <c r="I20" s="24"/>
       <c r="J20" s="26" t="s">
-        <v>677</v>
+        <v>676</v>
       </c>
       <c r="K20" s="24" t="s">
-        <v>808</v>
+        <v>807</v>
       </c>
       <c r="L20" s="25" t="s">
+        <v>778</v>
+      </c>
+      <c r="M20" s="24" t="s">
+        <v>777</v>
+      </c>
+      <c r="N20" s="24" t="s">
         <v>779</v>
-      </c>
-      <c r="M20" s="24" t="s">
-        <v>778</v>
-      </c>
-      <c r="N20" s="24" t="s">
-        <v>780</v>
       </c>
       <c r="O20" s="24"/>
       <c r="P20" s="24"/>
       <c r="Q20" s="24" t="s">
-        <v>786</v>
+        <v>785</v>
       </c>
       <c r="R20" s="24" t="s">
-        <v>687</v>
+        <v>686</v>
       </c>
       <c r="S20" s="24" t="s">
         <v>641</v>
@@ -5005,34 +5005,34 @@
         <v>642</v>
       </c>
       <c r="U20" s="24" t="s">
-        <v>718</v>
+        <v>717</v>
       </c>
       <c r="V20" s="24" t="s">
-        <v>801</v>
+        <v>800</v>
       </c>
       <c r="W20" s="24" t="s">
-        <v>808</v>
+        <v>807</v>
       </c>
       <c r="X20" s="24"/>
       <c r="Y20" s="24" t="s">
-        <v>803</v>
+        <v>802</v>
       </c>
     </row>
     <row r="21" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A21" s="24" t="s">
-        <v>709</v>
+        <v>708</v>
       </c>
       <c r="B21" s="28" t="s">
         <v>485</v>
       </c>
       <c r="C21" s="24" t="s">
-        <v>712</v>
+        <v>711</v>
       </c>
       <c r="D21" s="24" t="s">
         <v>384</v>
       </c>
       <c r="E21" s="24" t="s">
-        <v>715</v>
+        <v>714</v>
       </c>
       <c r="F21" s="24" t="s">
         <v>381</v>
@@ -5045,25 +5045,25 @@
       </c>
       <c r="I21" s="24"/>
       <c r="J21" s="12" t="s">
-        <v>791</v>
+        <v>790</v>
       </c>
       <c r="K21" s="24" t="s">
-        <v>790</v>
+        <v>789</v>
       </c>
       <c r="L21" s="25" t="s">
+        <v>718</v>
+      </c>
+      <c r="M21" s="24" t="s">
         <v>719</v>
       </c>
-      <c r="M21" s="24" t="s">
-        <v>720</v>
-      </c>
       <c r="N21" s="24" t="s">
-        <v>720</v>
+        <v>719</v>
       </c>
       <c r="O21" s="24"/>
       <c r="P21" s="24"/>
       <c r="Q21" s="24"/>
       <c r="R21" s="24" t="s">
-        <v>721</v>
+        <v>720</v>
       </c>
       <c r="S21" s="24" t="s">
         <v>641</v>
@@ -5072,34 +5072,34 @@
         <v>642</v>
       </c>
       <c r="U21" s="24" t="s">
-        <v>722</v>
+        <v>721</v>
       </c>
       <c r="V21" s="24" t="s">
-        <v>804</v>
+        <v>803</v>
       </c>
       <c r="W21" s="24" t="s">
-        <v>808</v>
+        <v>807</v>
       </c>
       <c r="X21" s="24"/>
       <c r="Y21" s="24" t="s">
-        <v>803</v>
+        <v>802</v>
       </c>
     </row>
     <row r="22" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A22" s="24" t="s">
-        <v>723</v>
+        <v>722</v>
       </c>
       <c r="B22" s="28" t="s">
         <v>485</v>
       </c>
       <c r="C22" s="24" t="s">
-        <v>724</v>
+        <v>723</v>
       </c>
       <c r="D22" s="24" t="s">
         <v>384</v>
       </c>
       <c r="E22" s="24" t="s">
-        <v>725</v>
+        <v>724</v>
       </c>
       <c r="F22" s="24" t="s">
         <v>381</v>
@@ -5114,27 +5114,27 @@
         <v>433</v>
       </c>
       <c r="J22" s="24" t="s">
-        <v>731</v>
+        <v>730</v>
       </c>
       <c r="K22" s="24" t="s">
-        <v>809</v>
+        <v>808</v>
       </c>
       <c r="L22" s="24" t="s">
-        <v>726</v>
+        <v>725</v>
       </c>
       <c r="M22" s="24" t="s">
+        <v>786</v>
+      </c>
+      <c r="N22" s="24" t="s">
         <v>787</v>
-      </c>
-      <c r="N22" s="24" t="s">
-        <v>788</v>
       </c>
       <c r="O22" s="24"/>
       <c r="P22" s="24"/>
       <c r="Q22" s="24" t="s">
-        <v>789</v>
+        <v>788</v>
       </c>
       <c r="R22" s="24" t="s">
-        <v>721</v>
+        <v>720</v>
       </c>
       <c r="S22" s="24" t="s">
         <v>641</v>
@@ -5143,28 +5143,28 @@
         <v>642</v>
       </c>
       <c r="U22" s="24" t="s">
-        <v>732</v>
+        <v>731</v>
       </c>
       <c r="V22" s="24" t="s">
-        <v>801</v>
+        <v>800</v>
       </c>
       <c r="W22" s="24" t="s">
-        <v>808</v>
+        <v>807</v>
       </c>
       <c r="X22" s="24"/>
       <c r="Y22" s="24" t="s">
-        <v>803</v>
+        <v>802</v>
       </c>
     </row>
     <row r="23" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A23" s="24" t="s">
-        <v>727</v>
+        <v>726</v>
       </c>
       <c r="B23" s="28" t="s">
         <v>485</v>
       </c>
       <c r="C23" s="24" t="s">
-        <v>729</v>
+        <v>728</v>
       </c>
       <c r="D23" s="24" t="s">
         <v>359</v>
@@ -5179,25 +5179,25 @@
       </c>
       <c r="I23" s="24"/>
       <c r="J23" s="25" t="s">
-        <v>795</v>
+        <v>794</v>
       </c>
       <c r="K23" s="24"/>
       <c r="L23" s="25" t="s">
+        <v>820</v>
+      </c>
+      <c r="M23" s="25" t="s">
+        <v>812</v>
+      </c>
+      <c r="N23" s="25" t="s">
         <v>821</v>
-      </c>
-      <c r="M23" s="25" t="s">
-        <v>813</v>
-      </c>
-      <c r="N23" s="25" t="s">
-        <v>822</v>
       </c>
       <c r="O23" s="24"/>
       <c r="P23" s="25" t="s">
-        <v>826</v>
+        <v>825</v>
       </c>
       <c r="Q23" s="24"/>
       <c r="R23" s="24" t="s">
-        <v>736</v>
+        <v>735</v>
       </c>
       <c r="S23" s="24" t="s">
         <v>641</v>
@@ -5209,23 +5209,23 @@
         <v>652</v>
       </c>
       <c r="V23" s="24" t="s">
-        <v>801</v>
+        <v>800</v>
       </c>
       <c r="W23" s="25"/>
       <c r="X23" s="24"/>
       <c r="Y23" s="24" t="s">
-        <v>806</v>
+        <v>805</v>
       </c>
     </row>
     <row r="24" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A24" s="24" t="s">
-        <v>728</v>
+        <v>727</v>
       </c>
       <c r="B24" s="28" t="s">
         <v>485</v>
       </c>
       <c r="C24" s="24" t="s">
-        <v>730</v>
+        <v>729</v>
       </c>
       <c r="D24" s="24" t="s">
         <v>359</v>
@@ -5240,25 +5240,25 @@
       </c>
       <c r="I24" s="24"/>
       <c r="J24" s="25" t="s">
-        <v>794</v>
+        <v>793</v>
       </c>
       <c r="K24" s="24"/>
       <c r="L24" s="25" t="s">
+        <v>820</v>
+      </c>
+      <c r="M24" s="25" t="s">
+        <v>812</v>
+      </c>
+      <c r="N24" s="25" t="s">
         <v>821</v>
-      </c>
-      <c r="M24" s="25" t="s">
-        <v>813</v>
-      </c>
-      <c r="N24" s="25" t="s">
-        <v>822</v>
       </c>
       <c r="O24" s="24"/>
       <c r="P24" s="25" t="s">
-        <v>827</v>
+        <v>826</v>
       </c>
       <c r="Q24" s="24"/>
       <c r="R24" s="24" t="s">
-        <v>736</v>
+        <v>735</v>
       </c>
       <c r="S24" s="24" t="s">
         <v>641</v>
@@ -5270,29 +5270,29 @@
         <v>653</v>
       </c>
       <c r="V24" s="24" t="s">
-        <v>801</v>
+        <v>800</v>
       </c>
       <c r="W24" s="25"/>
       <c r="X24" s="24"/>
       <c r="Y24" s="24" t="s">
-        <v>806</v>
+        <v>805</v>
       </c>
     </row>
     <row r="25" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A25" s="24" t="s">
-        <v>733</v>
+        <v>732</v>
       </c>
       <c r="B25" s="28" t="s">
         <v>485</v>
       </c>
       <c r="C25" s="24" t="s">
-        <v>737</v>
+        <v>736</v>
       </c>
       <c r="D25" s="24" t="s">
         <v>384</v>
       </c>
       <c r="E25" s="24" t="s">
-        <v>738</v>
+        <v>737</v>
       </c>
       <c r="F25" s="24" t="s">
         <v>381</v>
@@ -5307,27 +5307,27 @@
         <v>433</v>
       </c>
       <c r="J25" s="24" t="s">
-        <v>677</v>
+        <v>676</v>
       </c>
       <c r="K25" s="24" t="s">
-        <v>808</v>
+        <v>807</v>
       </c>
       <c r="L25" s="24" t="s">
+        <v>733</v>
+      </c>
+      <c r="M25" s="24" t="s">
         <v>734</v>
       </c>
-      <c r="M25" s="24" t="s">
-        <v>735</v>
-      </c>
       <c r="N25" s="24" t="s">
-        <v>768</v>
+        <v>767</v>
       </c>
       <c r="O25" s="24"/>
       <c r="P25" s="24"/>
       <c r="Q25" s="24" t="s">
-        <v>769</v>
+        <v>768</v>
       </c>
       <c r="R25" s="24" t="s">
-        <v>687</v>
+        <v>686</v>
       </c>
       <c r="S25" s="24" t="s">
         <v>641</v>
@@ -5336,34 +5336,34 @@
         <v>642</v>
       </c>
       <c r="U25" s="24" t="s">
-        <v>749</v>
+        <v>748</v>
       </c>
       <c r="V25" s="24" t="s">
-        <v>801</v>
+        <v>800</v>
       </c>
       <c r="W25" s="24" t="s">
-        <v>808</v>
+        <v>807</v>
       </c>
       <c r="X25" s="24"/>
       <c r="Y25" s="24" t="s">
-        <v>803</v>
+        <v>802</v>
       </c>
     </row>
     <row r="26" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A26" s="24" t="s">
-        <v>740</v>
+        <v>739</v>
       </c>
       <c r="B26" s="28" t="s">
         <v>485</v>
       </c>
       <c r="C26" s="24" t="s">
-        <v>741</v>
+        <v>740</v>
       </c>
       <c r="D26" s="24" t="s">
         <v>384</v>
       </c>
       <c r="E26" s="24" t="s">
-        <v>742</v>
+        <v>741</v>
       </c>
       <c r="F26" s="24" t="s">
         <v>381</v>
@@ -5376,24 +5376,24 @@
       </c>
       <c r="I26" s="24"/>
       <c r="J26" s="24" t="s">
-        <v>739</v>
+        <v>738</v>
       </c>
       <c r="K26" s="24" t="s">
-        <v>808</v>
+        <v>807</v>
       </c>
       <c r="L26" s="24" t="s">
-        <v>810</v>
+        <v>809</v>
       </c>
       <c r="M26" s="24" t="s">
-        <v>770</v>
+        <v>769</v>
       </c>
       <c r="N26" s="24" t="s">
-        <v>770</v>
+        <v>769</v>
       </c>
       <c r="O26" s="24"/>
       <c r="P26" s="24"/>
       <c r="Q26" s="24" t="s">
-        <v>771</v>
+        <v>770</v>
       </c>
       <c r="R26" s="24" t="s">
         <v>647</v>
@@ -5405,34 +5405,34 @@
         <v>642</v>
       </c>
       <c r="U26" s="24" t="s">
-        <v>744</v>
+        <v>743</v>
       </c>
       <c r="V26" s="24" t="s">
-        <v>801</v>
+        <v>800</v>
       </c>
       <c r="W26" s="24" t="s">
-        <v>808</v>
+        <v>807</v>
       </c>
       <c r="X26" s="24"/>
       <c r="Y26" s="24" t="s">
-        <v>803</v>
+        <v>802</v>
       </c>
     </row>
     <row r="27" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A27" s="24" t="s">
-        <v>743</v>
+        <v>742</v>
       </c>
       <c r="B27" s="28" t="s">
         <v>485</v>
       </c>
       <c r="C27" s="24" t="s">
-        <v>745</v>
+        <v>744</v>
       </c>
       <c r="D27" s="24" t="s">
         <v>384</v>
       </c>
       <c r="E27" s="24" t="s">
-        <v>750</v>
+        <v>749</v>
       </c>
       <c r="F27" s="24" t="s">
         <v>381</v>
@@ -5445,24 +5445,24 @@
       </c>
       <c r="I27" s="24"/>
       <c r="J27" s="24" t="s">
-        <v>747</v>
+        <v>746</v>
       </c>
       <c r="K27" s="24" t="s">
-        <v>808</v>
+        <v>807</v>
       </c>
       <c r="L27" s="24" t="s">
-        <v>746</v>
+        <v>745</v>
       </c>
       <c r="M27" s="24" t="s">
+        <v>771</v>
+      </c>
+      <c r="N27" s="24" t="s">
         <v>772</v>
-      </c>
-      <c r="N27" s="24" t="s">
-        <v>773</v>
       </c>
       <c r="O27" s="24"/>
       <c r="P27" s="24"/>
       <c r="Q27" s="24" t="s">
-        <v>777</v>
+        <v>776</v>
       </c>
       <c r="R27" s="24" t="s">
         <v>647</v>
@@ -5474,17 +5474,17 @@
         <v>642</v>
       </c>
       <c r="U27" s="24" t="s">
-        <v>748</v>
+        <v>747</v>
       </c>
       <c r="V27" s="24" t="s">
-        <v>804</v>
+        <v>803</v>
       </c>
       <c r="W27" s="24" t="s">
-        <v>808</v>
+        <v>807</v>
       </c>
       <c r="X27" s="24"/>
       <c r="Y27" s="24" t="s">
-        <v>803</v>
+        <v>802</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Wrangled OLR and CLR based on QA, ready for production
</commit_message>
<xml_diff>
--- a/villegas/OLR/OLR_villegas_mss0758.xlsx
+++ b/villegas/OLR/OLR_villegas_mss0758.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GitHub\domm-metadata\villegas\OLR\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Y:\_one_off\Villegas\Final_metadata\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -133,7 +133,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1153" uniqueCount="834">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1153" uniqueCount="835">
   <si>
     <t>text</t>
   </si>
@@ -2112,9 +2112,6 @@
     <t>Real del Monte mine - Legal agreements and contracts</t>
   </si>
   <si>
-    <t>Real del Monte mine</t>
-  </si>
-  <si>
     <t>m0758b03f015i001.tif</t>
   </si>
   <si>
@@ -2391,9 +2388,6 @@
     <t>1834-09-26</t>
   </si>
   <si>
-    <t>Letters from treasurer Samuel Notley (Mineral del Monte) to company manager John Taylor (London) on monthly expenditures and returns, from Henry A. Mackintosh to commissioner Charles Tindal about Henry Lorck and operations at Zimapan, and from commissioner Roderick Mackenzie to Diputados de la Mineria de Pachuca on labor issues. Also a report on company financials to Don Pedro Romero de Terreros, Conde de Regla.</t>
-  </si>
-  <si>
     <t>1854-05-13</t>
   </si>
   <si>
@@ -2424,18 +2418,12 @@
     <t>1863-02-22</t>
   </si>
   <si>
-    <t>Chiefly accounting and shipping correspondence from Edward Hay, Charles Whitehead, and William Rabling, with some letters about salt shipments from Texcoco to Hacienda de Loreto and iron furnished by the "ferrerias" of Encarnación and Guadalupe.  Contains May 1860 government notice extending Constitutionalist military aid and protection to mine properties and employees. Also December 1861 report (with English and Spanish versions) by Joseph Grose on the woods of Concepción and Capula, the latter having disputed rights. Government instructions regarding exports of company silver paste through Veracruz. Letter to Escandón on installation of metal milling machines at Guanajuato. A February 1862 letter from Whitehead mentions the foreign intervention, with troops marching to Córdoba, Orizaba, and Tehuacán.</t>
-  </si>
-  <si>
     <t>1857-10-03</t>
   </si>
   <si>
     <t>1857-1859</t>
   </si>
   <si>
-    <t>Reporting mine operations, damages caused by slag, employee changes, billing transactions, payment orders, salt from Texcoco. Letter from Thomas R. Auld on arrival of 250 "pronunciados" in the mine area, with  various other forces expected; three persons ("reos") removed by force from local presidio. Letters from Auld on machinery and other supplies held up in transit by government order; General Echeagaray is mentioned. Employment reference for John Noble, pitman, Tlalpujahua mining company. Notice on "numerous complaints of drunkenness and quarrelsome disorderly behaviour amongst the Englishment employed by this Company." Letter from Juan Basquez (Carcel Nacional, Pachuca) to Adrian Daste; letter to John H. Buchan from Francisco Hernandez and Jose Maria Medina.</t>
-  </si>
-  <si>
     <t>1829-04-07</t>
   </si>
   <si>
@@ -2586,15 +2574,6 @@
     <t>Casa de la máquina de vapor y chimenea Real del Monte</t>
   </si>
   <si>
-    <t>Real del Monte mine building</t>
-  </si>
-  <si>
-    <t>Real del Monte mine chimney</t>
-  </si>
-  <si>
-    <t>Compressor at "la Dificultad," Real del Monte mine</t>
-  </si>
-  <si>
     <t>between 1895 and 1945</t>
   </si>
   <si>
@@ -2635,6 +2614,30 @@
   </si>
   <si>
     <t>m0758b03f016.tif</t>
+  </si>
+  <si>
+    <t>Letters from treasurer Samuel Notley (Mineral del Monte) to company manager John Taylor (London) on monthly expenditures and returns, from Henry A. Mackintosh to commissioner Charles Tindal about Henry Lorck and operations at Zimapán, and from commissioner Roderick Mackenzie to Diputados de la Mineria de Pachuca on labor issues. Also a report on company financials to Don Pedro Romero de Terreros, Conde de Regla.</t>
+  </si>
+  <si>
+    <t>Chiefly accounting and shipping correspondence from Edward Hay, Charles Whitehead, and William Rabling, with some letters about salt shipments from Texcoco to Hacienda de Loreto and iron furnished by the "ferrerías" of Encarnación and Guadalupe.  Contains May 1860 government notice extending Constitutionalist military aid and protection to mine properties and employees. Also December 1861 report (with English and Spanish versions) by Joseph Grose on the woods of Concepción and Capula, the latter having disputed rights. Government instructions regarding exports of company silver paste through Veracruz. Letter to Manuel Escandón on installation of metal milling machines at Guanajuato. A February 1862 letter from Whitehead mentions the foreign intervention, with troops marching to Córdoba, Orizaba, and Tehuacán.</t>
+  </si>
+  <si>
+    <t>Reporting mine operations, damages caused by slag, employee changes, billing transactions, payment orders, salt from Texcoco. Letter from Thomas R. Auld on arrival of 250 "pronunciados" in the mine area, with  various other forces expected; three persons ("reos") removed by force from local presidio. Letters from Auld on machinery and other supplies held up in transit by government order; General Echeagaray is mentioned. Employment reference for John Noble, pitman, Tlalpujahua mining company. Notice on "numerous complaints of drunkenness and quarrelsome disorderly behaviour amongst the Englishment employed by this Company." Letter from Juan Basquez (Carcel Nacional, Pachuca) to Adrian Daste; letter to John H. Buchan from Francisco Hernandez and José María Medina.</t>
+  </si>
+  <si>
+    <t>Company of Adventurers in the Mines of Real del Monte</t>
+  </si>
+  <si>
+    <t>Hacienda de Beneficio Loreto, Pachuca, Hidalgo</t>
+  </si>
+  <si>
+    <t>Compressor at La Dificultad mine, Pachuca, Hidalgo</t>
+  </si>
+  <si>
+    <t>La Dificultad mine steam engine house, Pachuca, Hidalgo</t>
+  </si>
+  <si>
+    <t>La Dificultad mine steam engine house chimney, Pachuca, Hidalgo</t>
   </si>
 </sst>
 </file>
@@ -3681,7 +3684,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E12" sqref="E12"/>
+      <selection pane="bottomLeft" activeCell="V7" sqref="V7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3693,8 +3696,8 @@
     <col min="6" max="6" width="16.85546875" style="3" customWidth="1"/>
     <col min="7" max="7" width="16.28515625" style="3" bestFit="1" customWidth="1"/>
     <col min="8" max="9" width="22" style="3" customWidth="1"/>
-    <col min="10" max="10" width="51.5703125" style="3" customWidth="1"/>
-    <col min="11" max="11" width="32.7109375" style="3" customWidth="1"/>
+    <col min="10" max="10" width="59.140625" style="3" customWidth="1"/>
+    <col min="11" max="11" width="51.42578125" style="3" customWidth="1"/>
     <col min="12" max="12" width="25" style="3" customWidth="1"/>
     <col min="13" max="13" width="14.85546875" style="3" customWidth="1"/>
     <col min="14" max="14" width="15.140625" style="3" customWidth="1"/>
@@ -3804,17 +3807,17 @@
       </c>
       <c r="K2" s="24"/>
       <c r="L2" s="24" t="s">
-        <v>799</v>
+        <v>795</v>
       </c>
       <c r="M2" s="24" t="s">
-        <v>829</v>
+        <v>822</v>
       </c>
       <c r="N2" s="24" t="s">
-        <v>830</v>
+        <v>823</v>
       </c>
       <c r="O2" s="24"/>
       <c r="P2" s="25" t="s">
-        <v>810</v>
+        <v>806</v>
       </c>
       <c r="Q2" s="24"/>
       <c r="R2" s="24" t="s">
@@ -3828,12 +3831,12 @@
       </c>
       <c r="U2" s="24"/>
       <c r="V2" s="24" t="s">
-        <v>800</v>
+        <v>796</v>
       </c>
       <c r="W2" s="24"/>
       <c r="X2" s="24"/>
       <c r="Y2" s="24" t="s">
-        <v>801</v>
+        <v>797</v>
       </c>
     </row>
     <row r="3" spans="1:25" x14ac:dyDescent="0.25">
@@ -3841,7 +3844,7 @@
         <v>632</v>
       </c>
       <c r="B3" t="s">
-        <v>827</v>
+        <v>820</v>
       </c>
       <c r="C3" t="s">
         <v>634</v>
@@ -3884,7 +3887,7 @@
         <v>632</v>
       </c>
       <c r="B4" t="s">
-        <v>827</v>
+        <v>820</v>
       </c>
       <c r="C4" t="s">
         <v>635</v>
@@ -3954,21 +3957,21 @@
         <v>658</v>
       </c>
       <c r="K5" s="24" t="s">
-        <v>807</v>
+        <v>803</v>
       </c>
       <c r="L5" s="24" t="s">
         <v>646</v>
       </c>
       <c r="M5" s="24" t="s">
+        <v>751</v>
+      </c>
+      <c r="N5" s="24" t="s">
         <v>753</v>
-      </c>
-      <c r="N5" s="24" t="s">
-        <v>755</v>
       </c>
       <c r="O5" s="24"/>
       <c r="P5" s="24"/>
       <c r="Q5" s="24" t="s">
-        <v>797</v>
+        <v>793</v>
       </c>
       <c r="R5" s="24" t="s">
         <v>647</v>
@@ -3983,14 +3986,14 @@
         <v>648</v>
       </c>
       <c r="V5" s="24" t="s">
-        <v>800</v>
+        <v>796</v>
       </c>
       <c r="W5" s="24" t="s">
-        <v>807</v>
+        <v>803</v>
       </c>
       <c r="X5" s="24"/>
       <c r="Y5" s="24" t="s">
-        <v>802</v>
+        <v>798</v>
       </c>
     </row>
     <row r="6" spans="1:25" x14ac:dyDescent="0.25">
@@ -4016,23 +4019,23 @@
       </c>
       <c r="I6" s="24"/>
       <c r="J6" s="24" t="s">
-        <v>816</v>
+        <v>812</v>
       </c>
       <c r="K6" s="24"/>
       <c r="L6" s="24" t="s">
+        <v>807</v>
+      </c>
+      <c r="M6" s="24" t="s">
+        <v>808</v>
+      </c>
+      <c r="N6" s="24" t="s">
+        <v>809</v>
+      </c>
+      <c r="O6" s="24" t="s">
+        <v>815</v>
+      </c>
+      <c r="P6" s="25" t="s">
         <v>811</v>
-      </c>
-      <c r="M6" s="24" t="s">
-        <v>812</v>
-      </c>
-      <c r="N6" s="24" t="s">
-        <v>813</v>
-      </c>
-      <c r="O6" s="24" t="s">
-        <v>822</v>
-      </c>
-      <c r="P6" s="25" t="s">
-        <v>815</v>
       </c>
       <c r="Q6" s="24"/>
       <c r="R6" s="24" t="s">
@@ -4048,14 +4051,14 @@
         <v>652</v>
       </c>
       <c r="V6" s="24" t="s">
-        <v>800</v>
+        <v>796</v>
       </c>
       <c r="W6" s="24" t="s">
-        <v>807</v>
+        <v>803</v>
       </c>
       <c r="X6" s="24"/>
       <c r="Y6" s="24" t="s">
-        <v>806</v>
+        <v>802</v>
       </c>
     </row>
     <row r="7" spans="1:25" x14ac:dyDescent="0.25">
@@ -4081,23 +4084,23 @@
       </c>
       <c r="I7" s="24"/>
       <c r="J7" s="24" t="s">
-        <v>817</v>
+        <v>833</v>
       </c>
       <c r="K7" s="24"/>
       <c r="L7" s="24" t="s">
+        <v>807</v>
+      </c>
+      <c r="M7" s="24" t="s">
+        <v>808</v>
+      </c>
+      <c r="N7" s="24" t="s">
+        <v>809</v>
+      </c>
+      <c r="O7" s="24" t="s">
+        <v>791</v>
+      </c>
+      <c r="P7" s="25" t="s">
         <v>811</v>
-      </c>
-      <c r="M7" s="24" t="s">
-        <v>812</v>
-      </c>
-      <c r="N7" s="24" t="s">
-        <v>813</v>
-      </c>
-      <c r="O7" s="24" t="s">
-        <v>795</v>
-      </c>
-      <c r="P7" s="25" t="s">
-        <v>815</v>
       </c>
       <c r="Q7" s="24"/>
       <c r="R7" s="24" t="s">
@@ -4113,14 +4116,14 @@
         <v>653</v>
       </c>
       <c r="V7" s="24" t="s">
-        <v>800</v>
+        <v>796</v>
       </c>
       <c r="W7" s="24" t="s">
-        <v>807</v>
+        <v>803</v>
       </c>
       <c r="X7" s="24"/>
       <c r="Y7" s="24" t="s">
-        <v>806</v>
+        <v>802</v>
       </c>
     </row>
     <row r="8" spans="1:25" x14ac:dyDescent="0.25">
@@ -4146,23 +4149,23 @@
       </c>
       <c r="I8" s="26"/>
       <c r="J8" s="26" t="s">
-        <v>818</v>
+        <v>834</v>
       </c>
       <c r="K8" s="24"/>
       <c r="L8" s="24" t="s">
+        <v>807</v>
+      </c>
+      <c r="M8" s="24" t="s">
+        <v>808</v>
+      </c>
+      <c r="N8" s="24" t="s">
+        <v>809</v>
+      </c>
+      <c r="O8" s="26" t="s">
+        <v>792</v>
+      </c>
+      <c r="P8" s="25" t="s">
         <v>811</v>
-      </c>
-      <c r="M8" s="24" t="s">
-        <v>812</v>
-      </c>
-      <c r="N8" s="24" t="s">
-        <v>813</v>
-      </c>
-      <c r="O8" s="26" t="s">
-        <v>796</v>
-      </c>
-      <c r="P8" s="25" t="s">
-        <v>815</v>
       </c>
       <c r="Q8" s="26"/>
       <c r="R8" s="24" t="s">
@@ -4178,25 +4181,25 @@
         <v>654</v>
       </c>
       <c r="V8" s="24" t="s">
-        <v>800</v>
+        <v>796</v>
       </c>
       <c r="W8" s="24" t="s">
-        <v>807</v>
+        <v>803</v>
       </c>
       <c r="X8" s="24"/>
       <c r="Y8" s="24" t="s">
-        <v>806</v>
+        <v>802</v>
       </c>
     </row>
     <row r="9" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A9" s="24" t="s">
-        <v>662</v>
+        <v>661</v>
       </c>
       <c r="B9" s="28" t="s">
         <v>485</v>
       </c>
       <c r="C9" s="27" t="s">
-        <v>660</v>
+        <v>659</v>
       </c>
       <c r="D9" s="26" t="s">
         <v>359</v>
@@ -4211,23 +4214,23 @@
       </c>
       <c r="I9" s="26"/>
       <c r="J9" s="26" t="s">
-        <v>659</v>
+        <v>831</v>
       </c>
       <c r="K9" s="24"/>
       <c r="L9" s="24" t="s">
-        <v>811</v>
+        <v>807</v>
       </c>
       <c r="M9" s="24" t="s">
-        <v>812</v>
+        <v>808</v>
       </c>
       <c r="N9" s="24" t="s">
-        <v>813</v>
+        <v>809</v>
       </c>
       <c r="O9" s="27" t="s">
-        <v>823</v>
+        <v>816</v>
       </c>
       <c r="P9" s="25" t="s">
-        <v>814</v>
+        <v>810</v>
       </c>
       <c r="Q9" s="27"/>
       <c r="R9" s="24" t="s">
@@ -4240,28 +4243,28 @@
         <v>642</v>
       </c>
       <c r="U9" s="24" t="s">
-        <v>665</v>
+        <v>664</v>
       </c>
       <c r="V9" s="24" t="s">
-        <v>800</v>
+        <v>796</v>
       </c>
       <c r="W9" s="24" t="s">
-        <v>807</v>
+        <v>803</v>
       </c>
       <c r="X9" s="24"/>
       <c r="Y9" s="24" t="s">
-        <v>806</v>
+        <v>802</v>
       </c>
     </row>
     <row r="10" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A10" s="24" t="s">
-        <v>663</v>
+        <v>662</v>
       </c>
       <c r="B10" s="28" t="s">
         <v>485</v>
       </c>
       <c r="C10" s="27" t="s">
-        <v>661</v>
+        <v>660</v>
       </c>
       <c r="D10" s="26" t="s">
         <v>359</v>
@@ -4276,23 +4279,23 @@
       </c>
       <c r="I10" s="26"/>
       <c r="J10" s="12" t="s">
-        <v>819</v>
+        <v>832</v>
       </c>
       <c r="K10" s="24"/>
       <c r="L10" s="24" t="s">
-        <v>811</v>
+        <v>807</v>
       </c>
       <c r="M10" s="24" t="s">
-        <v>812</v>
+        <v>808</v>
       </c>
       <c r="N10" s="24" t="s">
-        <v>813</v>
+        <v>809</v>
       </c>
       <c r="O10" s="27" t="s">
-        <v>824</v>
+        <v>817</v>
       </c>
       <c r="P10" s="25" t="s">
-        <v>814</v>
+        <v>810</v>
       </c>
       <c r="Q10" s="27"/>
       <c r="R10" s="24" t="s">
@@ -4305,34 +4308,34 @@
         <v>642</v>
       </c>
       <c r="U10" s="24" t="s">
-        <v>666</v>
+        <v>665</v>
       </c>
       <c r="V10" s="24" t="s">
-        <v>804</v>
+        <v>800</v>
       </c>
       <c r="W10" s="24" t="s">
-        <v>807</v>
+        <v>803</v>
       </c>
       <c r="X10" s="24"/>
       <c r="Y10" s="24" t="s">
-        <v>806</v>
+        <v>802</v>
       </c>
     </row>
     <row r="11" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A11" s="24" t="s">
-        <v>667</v>
+        <v>666</v>
       </c>
       <c r="B11" s="28" t="s">
         <v>485</v>
       </c>
       <c r="C11" s="24" t="s">
-        <v>669</v>
+        <v>668</v>
       </c>
       <c r="D11" s="24" t="s">
         <v>384</v>
       </c>
       <c r="E11" s="24" t="s">
-        <v>833</v>
+        <v>826</v>
       </c>
       <c r="F11" s="24" t="s">
         <v>381</v>
@@ -4345,22 +4348,22 @@
       </c>
       <c r="I11" s="24"/>
       <c r="J11" s="24" t="s">
-        <v>791</v>
+        <v>787</v>
       </c>
       <c r="K11" s="24"/>
       <c r="L11" s="24" t="s">
-        <v>668</v>
+        <v>667</v>
       </c>
       <c r="M11" s="24" t="s">
-        <v>671</v>
+        <v>670</v>
       </c>
       <c r="N11" s="24" t="s">
-        <v>671</v>
+        <v>670</v>
       </c>
       <c r="O11" s="24"/>
       <c r="P11" s="24"/>
       <c r="Q11" s="24" t="s">
-        <v>792</v>
+        <v>788</v>
       </c>
       <c r="R11" s="24" t="s">
         <v>647</v>
@@ -4372,32 +4375,32 @@
         <v>642</v>
       </c>
       <c r="U11" s="24" t="s">
-        <v>670</v>
+        <v>669</v>
       </c>
       <c r="V11" s="24"/>
       <c r="W11" s="24"/>
       <c r="X11" s="24" t="s">
-        <v>832</v>
+        <v>825</v>
       </c>
       <c r="Y11" s="24" t="s">
-        <v>802</v>
+        <v>798</v>
       </c>
     </row>
     <row r="12" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A12" s="24" t="s">
-        <v>672</v>
+        <v>671</v>
       </c>
       <c r="B12" s="28" t="s">
         <v>485</v>
       </c>
       <c r="C12" s="24" t="s">
-        <v>674</v>
+        <v>673</v>
       </c>
       <c r="D12" s="24" t="s">
         <v>384</v>
       </c>
       <c r="E12" s="24" t="s">
-        <v>675</v>
+        <v>674</v>
       </c>
       <c r="F12" s="24" t="s">
         <v>381</v>
@@ -4412,27 +4415,27 @@
         <v>433</v>
       </c>
       <c r="J12" s="24" t="s">
+        <v>675</v>
+      </c>
+      <c r="K12" s="24" t="s">
+        <v>830</v>
+      </c>
+      <c r="L12" s="24" t="s">
         <v>676</v>
       </c>
-      <c r="K12" s="24" t="s">
-        <v>807</v>
-      </c>
-      <c r="L12" s="24" t="s">
-        <v>677</v>
-      </c>
       <c r="M12" s="24" t="s">
+        <v>749</v>
+      </c>
+      <c r="N12" s="24" t="s">
         <v>750</v>
-      </c>
-      <c r="N12" s="24" t="s">
-        <v>751</v>
       </c>
       <c r="O12" s="24"/>
       <c r="P12" s="24"/>
       <c r="Q12" s="24" t="s">
-        <v>752</v>
+        <v>827</v>
       </c>
       <c r="R12" s="24" t="s">
-        <v>686</v>
+        <v>685</v>
       </c>
       <c r="S12" s="24" t="s">
         <v>641</v>
@@ -4441,34 +4444,34 @@
         <v>642</v>
       </c>
       <c r="U12" s="24" t="s">
-        <v>673</v>
+        <v>672</v>
       </c>
       <c r="V12" s="24" t="s">
-        <v>800</v>
+        <v>796</v>
       </c>
       <c r="W12" s="24" t="s">
-        <v>807</v>
+        <v>803</v>
       </c>
       <c r="X12" s="24"/>
       <c r="Y12" s="24" t="s">
-        <v>802</v>
+        <v>798</v>
       </c>
     </row>
     <row r="13" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A13" s="24" t="s">
-        <v>678</v>
+        <v>677</v>
       </c>
       <c r="B13" s="28" t="s">
         <v>485</v>
       </c>
       <c r="C13" s="24" t="s">
-        <v>679</v>
+        <v>678</v>
       </c>
       <c r="D13" s="24" t="s">
         <v>384</v>
       </c>
       <c r="E13" s="24" t="s">
-        <v>681</v>
+        <v>680</v>
       </c>
       <c r="F13" s="24" t="s">
         <v>381</v>
@@ -4481,27 +4484,27 @@
       </c>
       <c r="I13" s="24"/>
       <c r="J13" s="25" t="s">
-        <v>680</v>
+        <v>679</v>
       </c>
       <c r="K13" s="24" t="s">
-        <v>807</v>
+        <v>803</v>
       </c>
       <c r="L13" s="24" t="s">
+        <v>682</v>
+      </c>
+      <c r="M13" s="24" t="s">
         <v>683</v>
       </c>
-      <c r="M13" s="24" t="s">
-        <v>684</v>
-      </c>
       <c r="N13" s="24" t="s">
-        <v>684</v>
+        <v>683</v>
       </c>
       <c r="O13" s="24"/>
       <c r="P13" s="24"/>
       <c r="Q13" s="24" t="s">
-        <v>754</v>
+        <v>752</v>
       </c>
       <c r="R13" s="24" t="s">
-        <v>686</v>
+        <v>685</v>
       </c>
       <c r="S13" s="24" t="s">
         <v>641</v>
@@ -4510,34 +4513,34 @@
         <v>642</v>
       </c>
       <c r="U13" s="24" t="s">
-        <v>687</v>
+        <v>686</v>
       </c>
       <c r="V13" s="24" t="s">
-        <v>800</v>
+        <v>796</v>
       </c>
       <c r="W13" s="24" t="s">
-        <v>807</v>
+        <v>803</v>
       </c>
       <c r="X13" s="24"/>
       <c r="Y13" s="24" t="s">
-        <v>802</v>
+        <v>798</v>
       </c>
     </row>
     <row r="14" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A14" s="24" t="s">
-        <v>682</v>
+        <v>681</v>
       </c>
       <c r="B14" s="28" t="s">
         <v>485</v>
       </c>
       <c r="C14" s="24" t="s">
-        <v>685</v>
+        <v>684</v>
       </c>
       <c r="D14" s="24" t="s">
         <v>384</v>
       </c>
       <c r="E14" s="24" t="s">
-        <v>828</v>
+        <v>821</v>
       </c>
       <c r="F14" s="24" t="s">
         <v>381</v>
@@ -4552,27 +4555,27 @@
         <v>358</v>
       </c>
       <c r="J14" s="24" t="s">
-        <v>676</v>
+        <v>675</v>
       </c>
       <c r="K14" s="24" t="s">
-        <v>807</v>
+        <v>803</v>
       </c>
       <c r="L14" s="24" t="s">
-        <v>757</v>
+        <v>755</v>
       </c>
       <c r="M14" s="24" t="s">
+        <v>754</v>
+      </c>
+      <c r="N14" s="24" t="s">
         <v>756</v>
-      </c>
-      <c r="N14" s="24" t="s">
-        <v>758</v>
       </c>
       <c r="O14" s="24"/>
       <c r="P14" s="24"/>
       <c r="Q14" s="24" t="s">
-        <v>759</v>
+        <v>757</v>
       </c>
       <c r="R14" s="24" t="s">
-        <v>686</v>
+        <v>685</v>
       </c>
       <c r="S14" s="24" t="s">
         <v>641</v>
@@ -4581,34 +4584,34 @@
         <v>642</v>
       </c>
       <c r="U14" s="24" t="s">
-        <v>688</v>
+        <v>687</v>
       </c>
       <c r="V14" s="24" t="s">
-        <v>800</v>
+        <v>796</v>
       </c>
       <c r="W14" s="24" t="s">
-        <v>807</v>
+        <v>803</v>
       </c>
       <c r="X14" s="24"/>
       <c r="Y14" s="24" t="s">
-        <v>802</v>
+        <v>798</v>
       </c>
     </row>
     <row r="15" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A15" s="24" t="s">
-        <v>689</v>
+        <v>688</v>
       </c>
       <c r="B15" s="28" t="s">
         <v>485</v>
       </c>
       <c r="C15" s="24" t="s">
-        <v>692</v>
+        <v>691</v>
       </c>
       <c r="D15" s="24" t="s">
         <v>384</v>
       </c>
       <c r="E15" s="24" t="s">
-        <v>695</v>
+        <v>694</v>
       </c>
       <c r="F15" s="24" t="s">
         <v>381</v>
@@ -4623,27 +4626,27 @@
         <v>358</v>
       </c>
       <c r="J15" s="24" t="s">
-        <v>676</v>
+        <v>675</v>
       </c>
       <c r="K15" s="24" t="s">
-        <v>807</v>
+        <v>803</v>
       </c>
       <c r="L15" s="24" t="s">
-        <v>765</v>
+        <v>762</v>
       </c>
       <c r="M15" s="24" t="s">
-        <v>764</v>
+        <v>761</v>
       </c>
       <c r="N15" s="24" t="s">
-        <v>831</v>
+        <v>824</v>
       </c>
       <c r="O15" s="24"/>
       <c r="P15" s="24"/>
       <c r="Q15" s="24" t="s">
-        <v>766</v>
+        <v>829</v>
       </c>
       <c r="R15" s="24" t="s">
-        <v>686</v>
+        <v>685</v>
       </c>
       <c r="S15" s="24" t="s">
         <v>641</v>
@@ -4652,34 +4655,34 @@
         <v>642</v>
       </c>
       <c r="U15" s="24" t="s">
-        <v>698</v>
+        <v>697</v>
       </c>
       <c r="V15" s="24" t="s">
-        <v>800</v>
+        <v>796</v>
       </c>
       <c r="W15" s="24" t="s">
-        <v>807</v>
+        <v>803</v>
       </c>
       <c r="X15" s="24"/>
       <c r="Y15" s="24" t="s">
-        <v>802</v>
+        <v>798</v>
       </c>
     </row>
     <row r="16" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A16" s="24" t="s">
-        <v>690</v>
+        <v>689</v>
       </c>
       <c r="B16" s="28" t="s">
         <v>485</v>
       </c>
       <c r="C16" s="24" t="s">
-        <v>693</v>
+        <v>692</v>
       </c>
       <c r="D16" s="24" t="s">
         <v>384</v>
       </c>
       <c r="E16" s="24" t="s">
-        <v>696</v>
+        <v>695</v>
       </c>
       <c r="F16" s="24" t="s">
         <v>381</v>
@@ -4694,27 +4697,27 @@
         <v>358</v>
       </c>
       <c r="J16" s="24" t="s">
-        <v>676</v>
+        <v>675</v>
       </c>
       <c r="K16" s="24" t="s">
-        <v>807</v>
+        <v>803</v>
       </c>
       <c r="L16" s="24" t="s">
-        <v>761</v>
+        <v>759</v>
       </c>
       <c r="M16" s="24" t="s">
+        <v>758</v>
+      </c>
+      <c r="N16" s="24" t="s">
         <v>760</v>
-      </c>
-      <c r="N16" s="24" t="s">
-        <v>762</v>
       </c>
       <c r="O16" s="24"/>
       <c r="P16" s="24"/>
       <c r="Q16" s="24" t="s">
-        <v>763</v>
+        <v>828</v>
       </c>
       <c r="R16" s="24" t="s">
-        <v>686</v>
+        <v>685</v>
       </c>
       <c r="S16" s="24" t="s">
         <v>641</v>
@@ -4723,34 +4726,34 @@
         <v>642</v>
       </c>
       <c r="U16" s="24" t="s">
-        <v>699</v>
+        <v>698</v>
       </c>
       <c r="V16" s="24" t="s">
-        <v>800</v>
+        <v>796</v>
       </c>
       <c r="W16" s="24" t="s">
-        <v>807</v>
+        <v>803</v>
       </c>
       <c r="X16" s="24"/>
       <c r="Y16" s="24" t="s">
-        <v>802</v>
+        <v>798</v>
       </c>
     </row>
     <row r="17" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A17" s="24" t="s">
-        <v>691</v>
+        <v>690</v>
       </c>
       <c r="B17" s="28" t="s">
         <v>485</v>
       </c>
       <c r="C17" s="25" t="s">
-        <v>694</v>
+        <v>693</v>
       </c>
       <c r="D17" s="24" t="s">
         <v>384</v>
       </c>
       <c r="E17" s="24" t="s">
-        <v>697</v>
+        <v>696</v>
       </c>
       <c r="F17" s="24" t="s">
         <v>381</v>
@@ -4765,27 +4768,27 @@
         <v>358</v>
       </c>
       <c r="J17" s="24" t="s">
-        <v>676</v>
+        <v>675</v>
       </c>
       <c r="K17" s="24" t="s">
-        <v>807</v>
+        <v>803</v>
       </c>
       <c r="L17" s="24" t="s">
-        <v>664</v>
+        <v>663</v>
       </c>
       <c r="M17" s="24" t="s">
-        <v>773</v>
+        <v>769</v>
       </c>
       <c r="N17" s="24" t="s">
-        <v>774</v>
+        <v>770</v>
       </c>
       <c r="O17" s="24"/>
       <c r="P17" s="24"/>
       <c r="Q17" s="24" t="s">
-        <v>775</v>
+        <v>771</v>
       </c>
       <c r="R17" s="24" t="s">
-        <v>686</v>
+        <v>685</v>
       </c>
       <c r="S17" s="24" t="s">
         <v>641</v>
@@ -4794,34 +4797,34 @@
         <v>642</v>
       </c>
       <c r="U17" s="24" t="s">
-        <v>700</v>
+        <v>699</v>
       </c>
       <c r="V17" s="24" t="s">
+        <v>799</v>
+      </c>
+      <c r="W17" s="24" t="s">
         <v>803</v>
-      </c>
-      <c r="W17" s="24" t="s">
-        <v>807</v>
       </c>
       <c r="X17" s="24"/>
       <c r="Y17" s="24" t="s">
-        <v>802</v>
+        <v>798</v>
       </c>
     </row>
     <row r="18" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A18" s="24" t="s">
-        <v>701</v>
+        <v>700</v>
       </c>
       <c r="B18" s="28" t="s">
         <v>485</v>
       </c>
       <c r="C18" s="24" t="s">
-        <v>703</v>
+        <v>702</v>
       </c>
       <c r="D18" s="24" t="s">
         <v>384</v>
       </c>
       <c r="E18" s="24" t="s">
-        <v>704</v>
+        <v>703</v>
       </c>
       <c r="F18" s="24" t="s">
         <v>381</v>
@@ -4836,27 +4839,27 @@
         <v>358</v>
       </c>
       <c r="J18" s="24" t="s">
-        <v>676</v>
+        <v>675</v>
       </c>
       <c r="K18" s="24" t="s">
-        <v>807</v>
+        <v>803</v>
       </c>
       <c r="L18" s="24" t="s">
-        <v>702</v>
+        <v>701</v>
       </c>
       <c r="M18" s="24" t="s">
-        <v>783</v>
+        <v>779</v>
       </c>
       <c r="N18" s="24" t="s">
-        <v>784</v>
+        <v>780</v>
       </c>
       <c r="O18" s="24"/>
       <c r="P18" s="24"/>
       <c r="Q18" s="24" t="s">
-        <v>798</v>
+        <v>794</v>
       </c>
       <c r="R18" s="24" t="s">
-        <v>686</v>
+        <v>685</v>
       </c>
       <c r="S18" s="24" t="s">
         <v>641</v>
@@ -4865,34 +4868,34 @@
         <v>642</v>
       </c>
       <c r="U18" s="24" t="s">
-        <v>705</v>
+        <v>704</v>
       </c>
       <c r="V18" s="24" t="s">
-        <v>800</v>
+        <v>796</v>
       </c>
       <c r="W18" s="24" t="s">
-        <v>807</v>
+        <v>803</v>
       </c>
       <c r="X18" s="24"/>
       <c r="Y18" s="24" t="s">
-        <v>802</v>
+        <v>798</v>
       </c>
     </row>
     <row r="19" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A19" s="24" t="s">
-        <v>706</v>
+        <v>705</v>
       </c>
       <c r="B19" s="28" t="s">
         <v>485</v>
       </c>
       <c r="C19" s="24" t="s">
-        <v>709</v>
+        <v>708</v>
       </c>
       <c r="D19" s="24" t="s">
         <v>384</v>
       </c>
       <c r="E19" s="24" t="s">
-        <v>712</v>
+        <v>711</v>
       </c>
       <c r="F19" s="24" t="s">
         <v>381</v>
@@ -4907,27 +4910,27 @@
         <v>358</v>
       </c>
       <c r="J19" s="24" t="s">
-        <v>676</v>
+        <v>675</v>
       </c>
       <c r="K19" s="24" t="s">
-        <v>807</v>
+        <v>803</v>
       </c>
       <c r="L19" s="25" t="s">
-        <v>715</v>
+        <v>714</v>
       </c>
       <c r="M19" s="24" t="s">
-        <v>780</v>
+        <v>776</v>
       </c>
       <c r="N19" s="24" t="s">
-        <v>781</v>
+        <v>777</v>
       </c>
       <c r="O19" s="24"/>
       <c r="P19" s="24"/>
       <c r="Q19" s="24" t="s">
-        <v>782</v>
+        <v>778</v>
       </c>
       <c r="R19" s="24" t="s">
-        <v>686</v>
+        <v>685</v>
       </c>
       <c r="S19" s="24" t="s">
         <v>641</v>
@@ -4936,34 +4939,34 @@
         <v>642</v>
       </c>
       <c r="U19" s="24" t="s">
-        <v>716</v>
+        <v>715</v>
       </c>
       <c r="V19" s="24" t="s">
-        <v>800</v>
+        <v>796</v>
       </c>
       <c r="W19" s="24" t="s">
-        <v>807</v>
+        <v>803</v>
       </c>
       <c r="X19" s="24"/>
       <c r="Y19" s="24" t="s">
-        <v>802</v>
+        <v>798</v>
       </c>
     </row>
     <row r="20" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A20" s="24" t="s">
-        <v>707</v>
+        <v>706</v>
       </c>
       <c r="B20" s="28" t="s">
         <v>485</v>
       </c>
       <c r="C20" s="24" t="s">
-        <v>710</v>
+        <v>709</v>
       </c>
       <c r="D20" s="24" t="s">
         <v>384</v>
       </c>
       <c r="E20" s="24" t="s">
-        <v>713</v>
+        <v>712</v>
       </c>
       <c r="F20" s="24" t="s">
         <v>381</v>
@@ -4976,27 +4979,27 @@
       </c>
       <c r="I20" s="24"/>
       <c r="J20" s="26" t="s">
-        <v>676</v>
+        <v>675</v>
       </c>
       <c r="K20" s="24" t="s">
-        <v>807</v>
+        <v>803</v>
       </c>
       <c r="L20" s="25" t="s">
-        <v>778</v>
+        <v>774</v>
       </c>
       <c r="M20" s="24" t="s">
-        <v>777</v>
+        <v>773</v>
       </c>
       <c r="N20" s="24" t="s">
-        <v>779</v>
+        <v>775</v>
       </c>
       <c r="O20" s="24"/>
       <c r="P20" s="24"/>
       <c r="Q20" s="24" t="s">
-        <v>785</v>
+        <v>781</v>
       </c>
       <c r="R20" s="24" t="s">
-        <v>686</v>
+        <v>685</v>
       </c>
       <c r="S20" s="24" t="s">
         <v>641</v>
@@ -5005,34 +5008,34 @@
         <v>642</v>
       </c>
       <c r="U20" s="24" t="s">
-        <v>717</v>
+        <v>716</v>
       </c>
       <c r="V20" s="24" t="s">
-        <v>800</v>
+        <v>796</v>
       </c>
       <c r="W20" s="24" t="s">
-        <v>807</v>
+        <v>803</v>
       </c>
       <c r="X20" s="24"/>
       <c r="Y20" s="24" t="s">
-        <v>802</v>
+        <v>798</v>
       </c>
     </row>
     <row r="21" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A21" s="24" t="s">
-        <v>708</v>
+        <v>707</v>
       </c>
       <c r="B21" s="28" t="s">
         <v>485</v>
       </c>
       <c r="C21" s="24" t="s">
-        <v>711</v>
+        <v>710</v>
       </c>
       <c r="D21" s="24" t="s">
         <v>384</v>
       </c>
       <c r="E21" s="24" t="s">
-        <v>714</v>
+        <v>713</v>
       </c>
       <c r="F21" s="24" t="s">
         <v>381</v>
@@ -5045,25 +5048,25 @@
       </c>
       <c r="I21" s="24"/>
       <c r="J21" s="12" t="s">
-        <v>790</v>
+        <v>786</v>
       </c>
       <c r="K21" s="24" t="s">
-        <v>789</v>
+        <v>785</v>
       </c>
       <c r="L21" s="25" t="s">
+        <v>717</v>
+      </c>
+      <c r="M21" s="24" t="s">
         <v>718</v>
       </c>
-      <c r="M21" s="24" t="s">
-        <v>719</v>
-      </c>
       <c r="N21" s="24" t="s">
-        <v>719</v>
+        <v>718</v>
       </c>
       <c r="O21" s="24"/>
       <c r="P21" s="24"/>
       <c r="Q21" s="24"/>
       <c r="R21" s="24" t="s">
-        <v>720</v>
+        <v>719</v>
       </c>
       <c r="S21" s="24" t="s">
         <v>641</v>
@@ -5072,34 +5075,34 @@
         <v>642</v>
       </c>
       <c r="U21" s="24" t="s">
-        <v>721</v>
+        <v>720</v>
       </c>
       <c r="V21" s="24" t="s">
+        <v>799</v>
+      </c>
+      <c r="W21" s="24" t="s">
         <v>803</v>
-      </c>
-      <c r="W21" s="24" t="s">
-        <v>807</v>
       </c>
       <c r="X21" s="24"/>
       <c r="Y21" s="24" t="s">
-        <v>802</v>
+        <v>798</v>
       </c>
     </row>
     <row r="22" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A22" s="24" t="s">
-        <v>722</v>
+        <v>721</v>
       </c>
       <c r="B22" s="28" t="s">
         <v>485</v>
       </c>
       <c r="C22" s="24" t="s">
-        <v>723</v>
+        <v>722</v>
       </c>
       <c r="D22" s="24" t="s">
         <v>384</v>
       </c>
       <c r="E22" s="24" t="s">
-        <v>724</v>
+        <v>723</v>
       </c>
       <c r="F22" s="24" t="s">
         <v>381</v>
@@ -5114,27 +5117,27 @@
         <v>433</v>
       </c>
       <c r="J22" s="24" t="s">
-        <v>730</v>
+        <v>729</v>
       </c>
       <c r="K22" s="24" t="s">
-        <v>808</v>
+        <v>804</v>
       </c>
       <c r="L22" s="24" t="s">
-        <v>725</v>
+        <v>724</v>
       </c>
       <c r="M22" s="24" t="s">
-        <v>786</v>
+        <v>782</v>
       </c>
       <c r="N22" s="24" t="s">
-        <v>787</v>
+        <v>783</v>
       </c>
       <c r="O22" s="24"/>
       <c r="P22" s="24"/>
       <c r="Q22" s="24" t="s">
-        <v>788</v>
+        <v>784</v>
       </c>
       <c r="R22" s="24" t="s">
-        <v>720</v>
+        <v>719</v>
       </c>
       <c r="S22" s="24" t="s">
         <v>641</v>
@@ -5143,28 +5146,28 @@
         <v>642</v>
       </c>
       <c r="U22" s="24" t="s">
-        <v>731</v>
+        <v>730</v>
       </c>
       <c r="V22" s="24" t="s">
-        <v>800</v>
+        <v>796</v>
       </c>
       <c r="W22" s="24" t="s">
-        <v>807</v>
+        <v>803</v>
       </c>
       <c r="X22" s="24"/>
       <c r="Y22" s="24" t="s">
-        <v>802</v>
+        <v>798</v>
       </c>
     </row>
     <row r="23" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A23" s="24" t="s">
-        <v>726</v>
+        <v>725</v>
       </c>
       <c r="B23" s="28" t="s">
         <v>485</v>
       </c>
       <c r="C23" s="24" t="s">
-        <v>728</v>
+        <v>727</v>
       </c>
       <c r="D23" s="24" t="s">
         <v>359</v>
@@ -5179,25 +5182,25 @@
       </c>
       <c r="I23" s="24"/>
       <c r="J23" s="25" t="s">
-        <v>794</v>
+        <v>790</v>
       </c>
       <c r="K23" s="24"/>
       <c r="L23" s="25" t="s">
-        <v>820</v>
+        <v>813</v>
       </c>
       <c r="M23" s="25" t="s">
-        <v>812</v>
+        <v>808</v>
       </c>
       <c r="N23" s="25" t="s">
-        <v>821</v>
+        <v>814</v>
       </c>
       <c r="O23" s="24"/>
       <c r="P23" s="25" t="s">
-        <v>825</v>
+        <v>818</v>
       </c>
       <c r="Q23" s="24"/>
       <c r="R23" s="24" t="s">
-        <v>735</v>
+        <v>734</v>
       </c>
       <c r="S23" s="24" t="s">
         <v>641</v>
@@ -5209,23 +5212,23 @@
         <v>652</v>
       </c>
       <c r="V23" s="24" t="s">
-        <v>800</v>
+        <v>796</v>
       </c>
       <c r="W23" s="25"/>
       <c r="X23" s="24"/>
       <c r="Y23" s="24" t="s">
-        <v>805</v>
+        <v>801</v>
       </c>
     </row>
     <row r="24" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A24" s="24" t="s">
-        <v>727</v>
+        <v>726</v>
       </c>
       <c r="B24" s="28" t="s">
         <v>485</v>
       </c>
       <c r="C24" s="24" t="s">
-        <v>729</v>
+        <v>728</v>
       </c>
       <c r="D24" s="24" t="s">
         <v>359</v>
@@ -5240,25 +5243,25 @@
       </c>
       <c r="I24" s="24"/>
       <c r="J24" s="25" t="s">
-        <v>793</v>
+        <v>789</v>
       </c>
       <c r="K24" s="24"/>
       <c r="L24" s="25" t="s">
-        <v>820</v>
+        <v>813</v>
       </c>
       <c r="M24" s="25" t="s">
-        <v>812</v>
+        <v>808</v>
       </c>
       <c r="N24" s="25" t="s">
-        <v>821</v>
+        <v>814</v>
       </c>
       <c r="O24" s="24"/>
       <c r="P24" s="25" t="s">
-        <v>826</v>
+        <v>819</v>
       </c>
       <c r="Q24" s="24"/>
       <c r="R24" s="24" t="s">
-        <v>735</v>
+        <v>734</v>
       </c>
       <c r="S24" s="24" t="s">
         <v>641</v>
@@ -5270,29 +5273,29 @@
         <v>653</v>
       </c>
       <c r="V24" s="24" t="s">
-        <v>800</v>
+        <v>796</v>
       </c>
       <c r="W24" s="25"/>
       <c r="X24" s="24"/>
       <c r="Y24" s="24" t="s">
-        <v>805</v>
+        <v>801</v>
       </c>
     </row>
     <row r="25" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A25" s="24" t="s">
-        <v>732</v>
+        <v>731</v>
       </c>
       <c r="B25" s="28" t="s">
         <v>485</v>
       </c>
       <c r="C25" s="24" t="s">
-        <v>736</v>
+        <v>735</v>
       </c>
       <c r="D25" s="24" t="s">
         <v>384</v>
       </c>
       <c r="E25" s="24" t="s">
-        <v>737</v>
+        <v>736</v>
       </c>
       <c r="F25" s="24" t="s">
         <v>381</v>
@@ -5307,27 +5310,27 @@
         <v>433</v>
       </c>
       <c r="J25" s="24" t="s">
-        <v>676</v>
+        <v>675</v>
       </c>
       <c r="K25" s="24" t="s">
-        <v>807</v>
+        <v>830</v>
       </c>
       <c r="L25" s="24" t="s">
+        <v>732</v>
+      </c>
+      <c r="M25" s="24" t="s">
         <v>733</v>
       </c>
-      <c r="M25" s="24" t="s">
-        <v>734</v>
-      </c>
       <c r="N25" s="24" t="s">
-        <v>767</v>
+        <v>763</v>
       </c>
       <c r="O25" s="24"/>
       <c r="P25" s="24"/>
       <c r="Q25" s="24" t="s">
-        <v>768</v>
+        <v>764</v>
       </c>
       <c r="R25" s="24" t="s">
-        <v>686</v>
+        <v>685</v>
       </c>
       <c r="S25" s="24" t="s">
         <v>641</v>
@@ -5336,34 +5339,34 @@
         <v>642</v>
       </c>
       <c r="U25" s="24" t="s">
-        <v>748</v>
+        <v>747</v>
       </c>
       <c r="V25" s="24" t="s">
-        <v>800</v>
+        <v>796</v>
       </c>
       <c r="W25" s="24" t="s">
-        <v>807</v>
+        <v>803</v>
       </c>
       <c r="X25" s="24"/>
       <c r="Y25" s="24" t="s">
-        <v>802</v>
+        <v>798</v>
       </c>
     </row>
     <row r="26" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A26" s="24" t="s">
-        <v>739</v>
+        <v>738</v>
       </c>
       <c r="B26" s="28" t="s">
         <v>485</v>
       </c>
       <c r="C26" s="24" t="s">
-        <v>740</v>
+        <v>739</v>
       </c>
       <c r="D26" s="24" t="s">
         <v>384</v>
       </c>
       <c r="E26" s="24" t="s">
-        <v>741</v>
+        <v>740</v>
       </c>
       <c r="F26" s="24" t="s">
         <v>381</v>
@@ -5376,24 +5379,24 @@
       </c>
       <c r="I26" s="24"/>
       <c r="J26" s="24" t="s">
-        <v>738</v>
+        <v>737</v>
       </c>
       <c r="K26" s="24" t="s">
-        <v>807</v>
+        <v>830</v>
       </c>
       <c r="L26" s="24" t="s">
-        <v>809</v>
+        <v>805</v>
       </c>
       <c r="M26" s="24" t="s">
-        <v>769</v>
+        <v>765</v>
       </c>
       <c r="N26" s="24" t="s">
-        <v>769</v>
+        <v>765</v>
       </c>
       <c r="O26" s="24"/>
       <c r="P26" s="24"/>
       <c r="Q26" s="24" t="s">
-        <v>770</v>
+        <v>766</v>
       </c>
       <c r="R26" s="24" t="s">
         <v>647</v>
@@ -5405,34 +5408,34 @@
         <v>642</v>
       </c>
       <c r="U26" s="24" t="s">
-        <v>743</v>
+        <v>742</v>
       </c>
       <c r="V26" s="24" t="s">
-        <v>800</v>
+        <v>796</v>
       </c>
       <c r="W26" s="24" t="s">
-        <v>807</v>
+        <v>803</v>
       </c>
       <c r="X26" s="24"/>
       <c r="Y26" s="24" t="s">
-        <v>802</v>
+        <v>798</v>
       </c>
     </row>
     <row r="27" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A27" s="24" t="s">
-        <v>742</v>
+        <v>741</v>
       </c>
       <c r="B27" s="28" t="s">
         <v>485</v>
       </c>
       <c r="C27" s="24" t="s">
-        <v>744</v>
+        <v>743</v>
       </c>
       <c r="D27" s="24" t="s">
         <v>384</v>
       </c>
       <c r="E27" s="24" t="s">
-        <v>749</v>
+        <v>748</v>
       </c>
       <c r="F27" s="24" t="s">
         <v>381</v>
@@ -5445,24 +5448,24 @@
       </c>
       <c r="I27" s="24"/>
       <c r="J27" s="24" t="s">
-        <v>746</v>
+        <v>745</v>
       </c>
       <c r="K27" s="24" t="s">
-        <v>807</v>
+        <v>830</v>
       </c>
       <c r="L27" s="24" t="s">
-        <v>745</v>
+        <v>744</v>
       </c>
       <c r="M27" s="24" t="s">
-        <v>771</v>
+        <v>767</v>
       </c>
       <c r="N27" s="24" t="s">
-        <v>772</v>
+        <v>768</v>
       </c>
       <c r="O27" s="24"/>
       <c r="P27" s="24"/>
       <c r="Q27" s="24" t="s">
-        <v>776</v>
+        <v>772</v>
       </c>
       <c r="R27" s="24" t="s">
         <v>647</v>
@@ -5474,17 +5477,17 @@
         <v>642</v>
       </c>
       <c r="U27" s="24" t="s">
-        <v>747</v>
+        <v>746</v>
       </c>
       <c r="V27" s="24" t="s">
+        <v>799</v>
+      </c>
+      <c r="W27" s="24" t="s">
         <v>803</v>
-      </c>
-      <c r="W27" s="24" t="s">
-        <v>807</v>
       </c>
       <c r="X27" s="24"/>
       <c r="Y27" s="24" t="s">
-        <v>802</v>
+        <v>798</v>
       </c>
     </row>
   </sheetData>

</xml_diff>